<commit_message>
MongoDB to Excel 2
</commit_message>
<xml_diff>
--- a/Excel.xlsx
+++ b/Excel.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -13,9 +13,11 @@
     <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
     <sheet name="Sheet4" sheetId="5" r:id="rId5"/>
     <sheet name="Sheet5" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet6" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="entries" localSheetId="5">Sheet5!$A$1:$N$4</definedName>
+    <definedName name="entries" localSheetId="6">Sheet6!$A$1:$AC$2</definedName>
     <definedName name="test_images" localSheetId="2">Sheet2!$A$1:$R$7</definedName>
     <definedName name="test_images" localSheetId="3">Sheet3!$A$1:$R$7</definedName>
     <definedName name="test_images" localSheetId="4">Sheet4!$A$1:$R$7</definedName>
@@ -53,9 +55,20 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" name="test_images" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="850" sourceFile="C:\Users\Zoe\Bachelor\test_images.csv" decimal="," thousands="." tab="0" comma="1">
-      <textFields count="18">
+  <connection id="2" name="entries1" type="6" refreshedVersion="6" background="1" saveData="1">
+    <textPr codePage="850" sourceFile="C:\Users\Zoe\Bachelor\entries.csv" decimal="," thousands="." tab="0" comma="1">
+      <textFields count="29">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
         <textField/>
         <textField/>
         <textField/>
@@ -77,7 +90,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="3" name="test_images1" type="6" refreshedVersion="6" background="1" saveData="1">
+  <connection id="3" name="test_images" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\Zoe\Bachelor\test_images.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="18">
         <textField/>
@@ -101,8 +114,8 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="4" name="test_images2" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="850" sourceFile="C:\Users\Zoe\Bachelor\test_images.csv" thousands=" " tab="0" comma="1">
+  <connection id="4" name="test_images1" type="6" refreshedVersion="6" background="1" saveData="1">
+    <textPr codePage="850" sourceFile="C:\Users\Zoe\Bachelor\test_images.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="18">
         <textField/>
         <textField/>
@@ -125,16 +138,40 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="5" name="users_under_40" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="850" sourceFile="C:\Users\Zoe\Bachelor\test_images.csv" decimal="," thousands="." comma="1">
-      <textFields count="3">
+  <connection id="5" name="test_images2" type="6" refreshedVersion="6" background="1" saveData="1">
+    <textPr codePage="850" sourceFile="C:\Users\Zoe\Bachelor\test_images.csv" thousands=" " tab="0" comma="1">
+      <textFields count="18">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
         <textField/>
         <textField/>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="6" name="users_under_401" type="6" refreshedVersion="6" background="1" saveData="1">
+  <connection id="6" name="users_under_40" type="6" refreshedVersion="6" background="1" saveData="1">
+    <textPr codePage="850" sourceFile="C:\Users\Zoe\Bachelor\test_images.csv" decimal="," thousands="." comma="1">
+      <textFields count="3">
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="7" name="users_under_401" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\Zoe\Bachelor\users_under_40.csv" thousands=" " tab="0" comma="1">
       <textFields count="3">
         <textField/>
@@ -147,7 +184,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="73">
   <si>
     <t>Name</t>
   </si>
@@ -306,6 +343,66 @@
   </si>
   <si>
     <t xml:space="preserve"> 0 29.556409018785587 29.556409018785587</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>test1_result</t>
+  </si>
+  <si>
+    <t>test1_quickly</t>
+  </si>
+  <si>
+    <t>test1_difficult</t>
+  </si>
+  <si>
+    <t>test1_comfortable</t>
+  </si>
+  <si>
+    <t>test1_like</t>
+  </si>
+  <si>
+    <t>test1_dislike</t>
+  </si>
+  <si>
+    <t>test2_result</t>
+  </si>
+  <si>
+    <t>test2_time</t>
+  </si>
+  <si>
+    <t>test2_easy</t>
+  </si>
+  <si>
+    <t>test2_quickly</t>
+  </si>
+  <si>
+    <t>test2_difficult</t>
+  </si>
+  <si>
+    <t>test2_comfortable</t>
+  </si>
+  <si>
+    <t>test2_like</t>
+  </si>
+  <si>
+    <t>test2_dislike</t>
+  </si>
+  <si>
+    <t>56ac95d42233f1dc2aa17eb7</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0 0 0</t>
+  </si>
+  <si>
+    <t>-147.5</t>
+  </si>
+  <si>
+    <t>ss</t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
 </sst>
 </file>
@@ -364,27 +461,31 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="users_under_40" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="users_under_40" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="users_under_40" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="users_under_40" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="test_images" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="test_images" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="test_images" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="test_images" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="test_images" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="test_images" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="entries" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="entries" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2252,7 +2353,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2361,4 +2462,192 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AC2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="22" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="12.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L1" t="s">
+        <v>46</v>
+      </c>
+      <c r="M1" t="s">
+        <v>36</v>
+      </c>
+      <c r="N1" t="s">
+        <v>54</v>
+      </c>
+      <c r="O1" t="s">
+        <v>48</v>
+      </c>
+      <c r="P1" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>55</v>
+      </c>
+      <c r="R1" t="s">
+        <v>56</v>
+      </c>
+      <c r="S1" t="s">
+        <v>57</v>
+      </c>
+      <c r="T1" t="s">
+        <v>58</v>
+      </c>
+      <c r="U1" t="s">
+        <v>59</v>
+      </c>
+      <c r="V1" t="s">
+        <v>60</v>
+      </c>
+      <c r="W1" t="s">
+        <v>61</v>
+      </c>
+      <c r="X1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" t="s">
+        <v>50</v>
+      </c>
+      <c r="K2">
+        <v>2</v>
+      </c>
+      <c r="L2" s="1">
+        <v>1.47666666666666E+16</v>
+      </c>
+      <c r="M2" t="s">
+        <v>69</v>
+      </c>
+      <c r="N2" t="s">
+        <v>70</v>
+      </c>
+      <c r="O2">
+        <v>6</v>
+      </c>
+      <c r="P2">
+        <v>2</v>
+      </c>
+      <c r="Q2">
+        <v>2</v>
+      </c>
+      <c r="S2">
+        <v>2</v>
+      </c>
+      <c r="V2" s="1">
+        <v>-1.06492759700353E+16</v>
+      </c>
+      <c r="W2">
+        <v>9</v>
+      </c>
+      <c r="X2">
+        <v>2</v>
+      </c>
+      <c r="Y2">
+        <v>2</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA2">
+        <v>2</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Function in separate file
</commit_message>
<xml_diff>
--- a/Excel.xlsx
+++ b/Excel.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="6"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
   </sheets>
   <definedNames>
     <definedName name="entries" localSheetId="5">Sheet5!$A$1:$N$4</definedName>
-    <definedName name="entries" localSheetId="6">Sheet6!$A$1:$AC$2</definedName>
+    <definedName name="entries" localSheetId="6">Sheet6!$A$1:$AC$15</definedName>
     <definedName name="test_images" localSheetId="2">Sheet2!$A$1:$R$7</definedName>
     <definedName name="test_images" localSheetId="3">Sheet3!$A$1:$R$7</definedName>
     <definedName name="test_images" localSheetId="4">Sheet4!$A$1:$R$7</definedName>
@@ -184,7 +184,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="96">
   <si>
     <t>Name</t>
   </si>
@@ -403,6 +403,75 @@
   </si>
   <si>
     <t>s</t>
+  </si>
+  <si>
+    <t>56ac9c972233f1dc2aa17ec0</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>56ac9cdfa6e62d0029ab67b6</t>
+  </si>
+  <si>
+    <t>56accf0c6cbabdfc1472b0dc</t>
+  </si>
+  <si>
+    <t>56acd68759f671c40e4a9074</t>
+  </si>
+  <si>
+    <t>56acd9938584f07025b14a71</t>
+  </si>
+  <si>
+    <t>56acdbf659e7f7341cbf50fd</t>
+  </si>
+  <si>
+    <t>56acdcbda3b8ebec07ae9daa</t>
+  </si>
+  <si>
+    <t>56acdefc11e52d64287f6d68</t>
+  </si>
+  <si>
+    <t>56ace0ccc7dc11f012e3da04</t>
+  </si>
+  <si>
+    <t>56ace2005329f068279cfac3</t>
+  </si>
+  <si>
+    <t>56ace3a08fe82410206d7e23</t>
+  </si>
+  <si>
+    <t>56adf71bd9b0d1ac0d403bff</t>
+  </si>
+  <si>
+    <t>56adfd0fdabb2b70021d45e4</t>
+  </si>
+  <si>
+    <t>Zoe</t>
+  </si>
+  <si>
+    <t>female</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 296.8372381064871 130.61823889713892 237.86549413094573</t>
+  </si>
+  <si>
+    <t>rfr</t>
+  </si>
+  <si>
+    <t>rfrfr</t>
+  </si>
+  <si>
+    <t>oooooo</t>
+  </si>
+  <si>
+    <t>oooooooooooo</t>
+  </si>
+  <si>
+    <t>oo</t>
   </si>
 </sst>
 </file>
@@ -2466,18 +2535,18 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC2"/>
+  <dimension ref="A1:AC15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
       <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -2486,8 +2555,8 @@
     <col min="10" max="10" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="55.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.140625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="12.7109375" bestFit="1" customWidth="1"/>
@@ -2501,7 +2570,7 @@
     <col min="25" max="25" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2596,55 +2665,398 @@
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="D2" t="s">
         <v>50</v>
       </c>
-      <c r="K2">
-        <v>2</v>
-      </c>
-      <c r="L2" s="1">
+      <c r="E2" t="s">
+        <v>74</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="V2" s="1"/>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D3" t="s">
+        <v>50</v>
+      </c>
+      <c r="K3">
+        <v>4</v>
+      </c>
+      <c r="L3" s="1">
         <v>1.47666666666666E+16</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M3" t="s">
         <v>69</v>
       </c>
-      <c r="N2" t="s">
+      <c r="P3">
+        <v>3</v>
+      </c>
+      <c r="Q3">
+        <v>3</v>
+      </c>
+      <c r="S3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K4">
+        <v>2</v>
+      </c>
+      <c r="L4" s="1">
+        <v>1.47666666666666E+16</v>
+      </c>
+      <c r="M4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D5" t="s">
+        <v>50</v>
+      </c>
+      <c r="K5">
+        <v>2</v>
+      </c>
+      <c r="L5" s="1">
+        <v>1.47666666666666E+16</v>
+      </c>
+      <c r="M5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D6" t="s">
+        <v>50</v>
+      </c>
+      <c r="K6">
+        <v>3</v>
+      </c>
+      <c r="L6" s="1">
+        <v>1.47666666666666E+16</v>
+      </c>
+      <c r="M6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D7" t="s">
+        <v>50</v>
+      </c>
+      <c r="K7">
+        <v>2</v>
+      </c>
+      <c r="L7" s="1">
+        <v>1.47666666666666E+16</v>
+      </c>
+      <c r="M7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D8" t="s">
+        <v>50</v>
+      </c>
+      <c r="K8">
+        <v>2</v>
+      </c>
+      <c r="L8" s="1">
+        <v>1.47666666666666E+16</v>
+      </c>
+      <c r="M8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>81</v>
+      </c>
+      <c r="D9" t="s">
+        <v>50</v>
+      </c>
+      <c r="K9">
+        <v>2</v>
+      </c>
+      <c r="L9" s="1">
+        <v>1.47666666666666E+16</v>
+      </c>
+      <c r="M9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>82</v>
+      </c>
+      <c r="D10" t="s">
+        <v>50</v>
+      </c>
+      <c r="K10">
+        <v>2</v>
+      </c>
+      <c r="L10" s="1">
+        <v>1.47666666666666E+16</v>
+      </c>
+      <c r="M10" t="s">
+        <v>69</v>
+      </c>
+      <c r="P10">
+        <v>2</v>
+      </c>
+      <c r="Q10">
+        <v>2</v>
+      </c>
+      <c r="S10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>83</v>
+      </c>
+      <c r="D11" t="s">
+        <v>50</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11" s="1">
+        <v>1.47666666666666E+16</v>
+      </c>
+      <c r="M11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>84</v>
+      </c>
+      <c r="D12" t="s">
+        <v>50</v>
+      </c>
+      <c r="K12">
+        <v>2</v>
+      </c>
+      <c r="L12" s="1">
+        <v>1.47666666666666E+16</v>
+      </c>
+      <c r="M12" t="s">
+        <v>69</v>
+      </c>
+      <c r="P12">
+        <v>2</v>
+      </c>
+      <c r="Q12">
+        <v>2</v>
+      </c>
+      <c r="S12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>68</v>
+      </c>
+      <c r="D13" t="s">
+        <v>50</v>
+      </c>
+      <c r="K13">
+        <v>2</v>
+      </c>
+      <c r="L13" s="1">
+        <v>1.47666666666666E+16</v>
+      </c>
+      <c r="M13" t="s">
+        <v>69</v>
+      </c>
+      <c r="N13" t="s">
         <v>70</v>
       </c>
-      <c r="O2">
+      <c r="O13">
         <v>6</v>
       </c>
-      <c r="P2">
-        <v>2</v>
-      </c>
-      <c r="Q2">
-        <v>2</v>
-      </c>
-      <c r="S2">
-        <v>2</v>
-      </c>
-      <c r="V2" s="1">
+      <c r="P13">
+        <v>2</v>
+      </c>
+      <c r="Q13">
+        <v>2</v>
+      </c>
+      <c r="S13">
+        <v>2</v>
+      </c>
+      <c r="V13" s="1">
         <v>-1.06492759700353E+16</v>
       </c>
-      <c r="W2">
+      <c r="W13">
         <v>9</v>
       </c>
-      <c r="X2">
-        <v>2</v>
-      </c>
-      <c r="Y2">
-        <v>2</v>
-      </c>
-      <c r="Z2" t="s">
+      <c r="X13">
+        <v>2</v>
+      </c>
+      <c r="Y13">
+        <v>2</v>
+      </c>
+      <c r="Z13" t="s">
         <v>71</v>
       </c>
-      <c r="AA2">
-        <v>2</v>
-      </c>
-      <c r="AB2" t="s">
+      <c r="AA13">
+        <v>2</v>
+      </c>
+      <c r="AB13" t="s">
         <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>85</v>
+      </c>
+      <c r="D14" t="s">
+        <v>50</v>
+      </c>
+      <c r="K14">
+        <v>1</v>
+      </c>
+      <c r="L14" s="1">
+        <v>1.47666666666666E+16</v>
+      </c>
+      <c r="M14" t="s">
+        <v>69</v>
+      </c>
+      <c r="N14">
+        <v>282</v>
+      </c>
+      <c r="O14">
+        <v>6</v>
+      </c>
+      <c r="P14">
+        <v>2</v>
+      </c>
+      <c r="Q14">
+        <v>2</v>
+      </c>
+      <c r="S14">
+        <v>2</v>
+      </c>
+      <c r="V14" s="1">
+        <v>2.02582897685298E+16</v>
+      </c>
+      <c r="W14">
+        <v>21</v>
+      </c>
+      <c r="X14">
+        <v>2</v>
+      </c>
+      <c r="Y14">
+        <v>2</v>
+      </c>
+      <c r="AA14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>86</v>
+      </c>
+      <c r="B15" t="s">
+        <v>87</v>
+      </c>
+      <c r="C15">
+        <v>56</v>
+      </c>
+      <c r="D15" t="s">
+        <v>88</v>
+      </c>
+      <c r="E15" t="s">
+        <v>89</v>
+      </c>
+      <c r="G15">
+        <v>2</v>
+      </c>
+      <c r="H15">
+        <v>2</v>
+      </c>
+      <c r="I15">
+        <v>2</v>
+      </c>
+      <c r="J15">
+        <v>4</v>
+      </c>
+      <c r="K15">
+        <v>9</v>
+      </c>
+      <c r="L15" s="1">
+        <v>1.45028164446764E+16</v>
+      </c>
+      <c r="M15" t="s">
+        <v>90</v>
+      </c>
+      <c r="N15" s="1">
+        <v>2269314070043620</v>
+      </c>
+      <c r="O15">
+        <v>17</v>
+      </c>
+      <c r="P15">
+        <v>3</v>
+      </c>
+      <c r="Q15">
+        <v>3</v>
+      </c>
+      <c r="R15" t="s">
+        <v>91</v>
+      </c>
+      <c r="S15">
+        <v>3</v>
+      </c>
+      <c r="T15" t="s">
+        <v>92</v>
+      </c>
+      <c r="U15" t="s">
+        <v>92</v>
+      </c>
+      <c r="V15" s="1">
+        <v>2.1715208450784E+16</v>
+      </c>
+      <c r="W15">
+        <v>20</v>
+      </c>
+      <c r="X15">
+        <v>4</v>
+      </c>
+      <c r="Y15">
+        <v>4</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>93</v>
+      </c>
+      <c r="AA15">
+        <v>4</v>
+      </c>
+      <c r="AB15" t="s">
+        <v>94</v>
+      </c>
+      <c r="AC15" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>